<commit_message>
cleaned up data files and wrote README
</commit_message>
<xml_diff>
--- a/data/20220718_size-distribution.xlsx
+++ b/data/20220718_size-distribution.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerzeigler/Documents/projects/apatite-nano-ct/apatite-project-git/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerzeigler/Documents/apatite-nano-ct/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1422438B-F48B-1A48-A6CE-9C4148D458C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265A2A56-CEEC-424F-A981-62CC24DE9822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="2000" windowWidth="26240" windowHeight="15440" xr2:uid="{6563B874-FC3A-FD43-BB30-2B94A84D2818}"/>
   </bookViews>
   <sheets>
-    <sheet name="apatite" sheetId="1" r:id="rId1"/>
-    <sheet name="zircon" sheetId="2" r:id="rId2"/>
+    <sheet name="size" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029" iterate="1" concurrentCalc="0"/>
   <extLst>
@@ -36,12 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>z_obs_w_max</t>
+    <t>zircon_obs_w_max</t>
   </si>
   <si>
-    <t>a_obs_w_max</t>
+    <t>apatite_obs_w_max</t>
   </si>
 </sst>
 </file>
@@ -402,7 +401,7 @@
   <dimension ref="A1:B1099"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8165,24 +8164,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98EF6B3-858E-8140-9632-1E718F0399CC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>